<commit_message>
TP#20088: Freight and SmartPost WIP
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/IMPB SmartPost Returns.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/IMPB SmartPost Returns.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="85">
   <si>
     <t>ProcessShipmentRequest</t>
   </si>
@@ -130,9 +130,6 @@
     <t>Units</t>
   </si>
   <si>
-    <t>RequestedShipment</t>
-  </si>
-  <si>
     <t>PackagingType</t>
   </si>
   <si>
@@ -250,10 +247,37 @@
     <t>ProcessShipmentRequest.RequestedShipment.SpecialServicesRequested.ReturnShipmentDetail.Rma</t>
   </si>
   <si>
-    <t>ProcessShipmentRequest.RequestedShipment.SmartPostDetail</t>
-  </si>
-  <si>
     <t>SaveLabel</t>
+  </si>
+  <si>
+    <t>Recipient.Contact</t>
+  </si>
+  <si>
+    <t>ProcessShipmentRequest.RequestedPackageLineItems</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>ProcessShipmentRequest.RequestedShipment.RequestedPackageLineItems.SmartPostDetail</t>
+  </si>
+  <si>
+    <t>ProcessShipmentRequest.RequestedShipment.ShippingChargesPayment.Payor.ResponsibleParty.Address</t>
   </si>
 </sst>
 </file>
@@ -486,7 +510,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -713,6 +737,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="364">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1080,7 +1117,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="1" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1177,6 +1214,21 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="13" xfId="360" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="360" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="7" borderId="18" xfId="360" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="7" borderId="0" xfId="360" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="7" borderId="5" xfId="360" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="13" xfId="360" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1867,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BT25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3683,11 +3735,11 @@
   <sheetData>
     <row r="1" spans="1:72" s="3" customFormat="1" ht="219.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="23" t="s">
         <v>15</v>
@@ -3702,40 +3754,40 @@
         <v>11</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="J1" s="23" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>30</v>
@@ -3744,75 +3796,83 @@
         <v>30</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC1" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD1" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE1" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC1" s="23" t="s">
+      <c r="AF1" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="AD1" s="23" t="s">
+      <c r="AG1" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH1" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI1" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="AE1" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF1" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG1" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH1" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="AI1" s="23" t="s">
-        <v>62</v>
-      </c>
       <c r="AJ1" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AK1" s="23" t="s">
         <v>28</v>
       </c>
       <c r="AL1" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM1" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN1" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO1" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="AP1" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ1" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AM1" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="AN1" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="AO1" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="AP1" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="AQ1" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="AR1" s="2"/>
-      <c r="AS1" s="2"/>
-      <c r="AT1" s="2"/>
-      <c r="AU1" s="2"/>
+      <c r="AS1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT1" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU1" s="33" t="s">
+        <v>76</v>
+      </c>
       <c r="AV1" s="2"/>
       <c r="AW1" s="2"/>
       <c r="AX1" s="2"/>
@@ -3854,13 +3914,13 @@
         <v>23</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="21" t="s">
         <v>36</v>
-      </c>
-      <c r="J2" s="21" t="s">
-        <v>37</v>
       </c>
       <c r="K2" s="21" t="s">
         <v>24</v>
@@ -3926,13 +3986,13 @@
         <v>29</v>
       </c>
       <c r="AF2" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AG2" s="21" t="s">
         <v>31</v>
       </c>
       <c r="AH2" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AI2" s="21" t="s">
         <v>34</v>
@@ -3941,19 +4001,19 @@
         <v>13</v>
       </c>
       <c r="AK2" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AL2" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM2" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="AM2" s="21" t="s">
+      <c r="AN2" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="AN2" s="21" t="s">
-        <v>49</v>
-      </c>
       <c r="AO2" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AP2" s="21" t="s">
         <v>12</v>
@@ -3961,10 +4021,18 @@
       <c r="AQ2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="AR2" s="2"/>
-      <c r="AS2" s="2"/>
-      <c r="AT2" s="2"/>
-      <c r="AU2" s="2"/>
+      <c r="AR2" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="AS2" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT2" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="AU2" s="26" t="s">
+        <v>79</v>
+      </c>
       <c r="AV2" s="2"/>
       <c r="AW2" s="2"/>
       <c r="AX2" s="2"/>
@@ -3991,37 +4059,37 @@
       <c r="BS2" s="2"/>
       <c r="BT2" s="2"/>
     </row>
-    <row r="3" spans="1:72" s="5" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:72" s="5" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="b">
         <v>1</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>66</v>
+      <c r="B3" s="38" t="s">
+        <v>65</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="7">
         <v>510158040</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>2</v>
@@ -4048,11 +4116,11 @@
         <v>0</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="U3" s="8"/>
       <c r="V3" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="W3" s="10" t="s">
         <v>7</v>
@@ -4079,17 +4147,17 @@
         <v>510158040</v>
       </c>
       <c r="AE3" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AF3" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AG3" s="10"/>
       <c r="AH3" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AI3" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AJ3" s="10">
         <v>3</v>
@@ -4098,7 +4166,7 @@
         <v>1</v>
       </c>
       <c r="AL3" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AM3" s="10"/>
       <c r="AN3" s="10">
@@ -4107,10 +4175,18 @@
       <c r="AO3" s="10"/>
       <c r="AP3" s="10"/>
       <c r="AQ3" s="12"/>
-      <c r="AR3" s="3"/>
-      <c r="AS3" s="3"/>
-      <c r="AT3" s="3"/>
-      <c r="AU3" s="3"/>
+      <c r="AR3" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="AS3" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT3" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="AU3" s="36" t="s">
+        <v>82</v>
+      </c>
       <c r="AV3" s="3"/>
       <c r="AW3" s="3"/>
       <c r="AX3" s="3"/>
@@ -4141,31 +4217,31 @@
       <c r="A4" s="27" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="13">
         <v>510158040</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J4" s="16" t="s">
         <v>1</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L4" s="15" t="s">
         <v>2</v>
@@ -4192,11 +4268,11 @@
         <v>0</v>
       </c>
       <c r="T4" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="U4" s="14"/>
       <c r="V4" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="W4" s="16" t="s">
         <v>7</v>
@@ -4223,17 +4299,17 @@
         <v>510158040</v>
       </c>
       <c r="AE4" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AF4" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AG4" s="16"/>
       <c r="AH4" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AI4" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AJ4" s="16">
         <v>3</v>
@@ -4242,25 +4318,33 @@
         <v>1</v>
       </c>
       <c r="AL4" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AM4" s="16"/>
       <c r="AN4" s="16">
         <v>5531</v>
       </c>
       <c r="AO4" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AP4" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AQ4" s="18">
         <v>1234567</v>
       </c>
-      <c r="AR4" s="4"/>
-      <c r="AS4" s="4"/>
-      <c r="AT4" s="4"/>
-      <c r="AU4" s="4"/>
+      <c r="AR4" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="AS4" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT4" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="AU4" s="36" t="s">
+        <v>82</v>
+      </c>
       <c r="AV4" s="4"/>
       <c r="AW4" s="4"/>
       <c r="AX4" s="4"/>

</xml_diff>